<commit_message>
Aba de skills criada e algumas mudanças básicas no css.
</commit_message>
<xml_diff>
--- a/funcionarios.xlsx
+++ b/funcionarios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>banana</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
 </sst>
 </file>
@@ -451,10 +448,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -470,7 +467,7 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
         <v>10</v>
       </c>
       <c r="D3">

</xml_diff>